<commit_message>
add an example in sample sheet
</commit_message>
<xml_diff>
--- a/examples/TranslationCheckerTest_BulkAppTranslation.xlsx
+++ b/examples/TranslationCheckerTest_BulkAppTranslation.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cody Stahl\Documents\GitHub\CommcareTranslationChecker\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Modules_and_forms" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,12 @@
     <sheet name="module1_form3" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -174,30 +174,6 @@
   </si>
   <si>
     <t>Nombre</t>
-  </si>
-  <si>
-    <t>What color is your car?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>¿</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Que color es su coche?</t>
-    </r>
   </si>
   <si>
     <r>
@@ -302,11 +278,35 @@
   <si>
     <t>You drive a &lt;output value="/data/car_color"/&gt; &lt;output value="/data/car_model"/&gt;. Is this correct!?</t>
   </si>
+  <si>
+    <t>What color is **your** car?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>¿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Que color es **su ** coche?</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,7 +376,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{A6379CDD-B520-476A-BF71-CD9C27C1B1F8}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -676,21 +676,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -736,7 +736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -753,7 +753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -770,7 +770,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -787,39 +787,44 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="I6" t="s">
         <v>62</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -833,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -847,7 +852,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -863,23 +868,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="90.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -908,7 +918,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -916,32 +926,32 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -949,39 +959,44 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1010,33 +1025,38 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1065,44 +1085,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="56">
+      <c r="A3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC89AA7D-5C38-4D30-96C0-5361F9470A76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1133,5 +1158,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>